<commit_message>
VALID INVALID ERROR FIXED
</commit_message>
<xml_diff>
--- a/Review_sheet.xlsx
+++ b/Review_sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="123820"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rish\Documents\GitHub_Repositories\Review_Scraper_Streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9778665D-4DAD-40C0-8C90-4BD1B51CBC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A280B6-2C0F-444F-9145-D0DF49F88327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17126" uniqueCount="4722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16600" uniqueCount="4541">
   <si>
     <t>Enter review link here</t>
   </si>
@@ -13662,549 +13662,6 @@
   </si>
   <si>
     <t>https://www.flipkart.com/reviews/SMWGVCMGEXFVDZ2P:10?reviewId=207dd198-ec7a-4e94-a3fc-5efb71866291</t>
-  </si>
-  <si>
-    <t>review/B0CN2JC9HC/R3RB8ZXF73QQGR</t>
-  </si>
-  <si>
-    <t>Mohd Areeb</t>
-  </si>
-  <si>
-    <t>Verified Purchase</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 22 January 2024</t>
-  </si>
-  <si>
-    <t>boAt Engima X700 Smart Watch with 1.52” AMOLED Display,Premium Metal Body Design &amp; Functional Crown,Advanced BT Calling,200+ Cloud Watch Faces,World Clock, HR &amp; SpO2,IP67(Copper Blue)</t>
-  </si>
-  <si>
-    <t>worth in this price</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>review/B0CN2SYX6Q/R1E925UDIIOA9H</t>
-  </si>
-  <si>
-    <t>Mbappe</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 26 January 2024</t>
-  </si>
-  <si>
-    <t>boAt Engima X700 Smart Watch with 1.52” AMOLED Display,Premium Metal Body Design &amp; Functional Crown,Advanced BT Calling,200+ Cloud Watch Faces,World Clock, HR &amp; SpO2,IP67(Silver Chrome)</t>
-  </si>
-  <si>
-    <t>review/B0CN2JC9HC/R5L3CQLR2A1DB</t>
-  </si>
-  <si>
-    <t>mcstan</t>
-  </si>
-  <si>
-    <t>value of money 🤑</t>
-  </si>
-  <si>
-    <t>R1Q7ISLIJIY1D</t>
-  </si>
-  <si>
-    <t>Naveen kumar</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 20 January 2024</t>
-  </si>
-  <si>
-    <t>boAt Engima X700 Smart Watch with 1.52” AMOLED Display,Premium Metal Body Design &amp; Functional Crown,Advanced BT Calling, 200+ Cloud Watch Faces,World Clock, HR &amp; SpO2,IP67(Copper Black)</t>
-  </si>
-  <si>
-    <t>Perfect blend of class and comfort.</t>
-  </si>
-  <si>
-    <t>review/B0CN2N8H94/R3JFF3DNUAMKO5</t>
-  </si>
-  <si>
-    <t>Rahim</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 19 January 2024</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>R33VB6RNOFCEWT</t>
-  </si>
-  <si>
-    <t>Bhavay johar</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 23 January 2024</t>
-  </si>
-  <si>
-    <t>Best watch under best budget</t>
-  </si>
-  <si>
-    <t>review/B0CN2N8H94/R34IXO76ESG7IB</t>
-  </si>
-  <si>
-    <t>Rutik</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 25 January 2024</t>
-  </si>
-  <si>
-    <t>Good one!</t>
-  </si>
-  <si>
-    <t>1US2XEMAL3EB</t>
-  </si>
-  <si>
-    <t>Pradeep</t>
-  </si>
-  <si>
-    <t>Premium Quality Watch</t>
-  </si>
-  <si>
-    <t>R2OXCVVITRGETY</t>
-  </si>
-  <si>
-    <t>Sumant kumar</t>
-  </si>
-  <si>
-    <t>Value for Money</t>
-  </si>
-  <si>
-    <t>tps://www.amazon.in/gp/f.html?C=ETSVHW0T0C3M&amp;K=2RALHA32FWMPU&amp;M=urn:rtn:msg:20240124195822c72d6d052acb4ccd9814462258b0p0eu&amp;R=1EAU6PM73H558&amp;T=C&amp;U=https%3A%2F%2Fwww.amazon.in%2Freview%2FRLI7VVGSYFLM8%2Fref%3Dpe_1640331_66412301_cm_rv_eml_rv0_rv&amp;H=6C7HRHKFVSMQ2WIL7GAPOS2WJLCA&amp;ref_=pe_1640331_66412301_cm_rv_eml_rv0_rv</t>
-  </si>
-  <si>
-    <t>Ravi Koshti</t>
-  </si>
-  <si>
-    <t>Quality Product By Indian Brand</t>
-  </si>
-  <si>
-    <t>review/B0CN2N8H94/RYCZ8FM5RR98M</t>
-  </si>
-  <si>
-    <t>Ashraf Khan</t>
-  </si>
-  <si>
-    <t>A Premium Smartwatch</t>
-  </si>
-  <si>
-    <t>R2OPUHV924HLK4</t>
-  </si>
-  <si>
-    <t>Shashank Singhal</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 2 February 2024</t>
-  </si>
-  <si>
-    <t>Party wear smart watch</t>
-  </si>
-  <si>
-    <t>review/B0CN2N8H94/R3V4EQH0TYU37M</t>
-  </si>
-  <si>
-    <t>Ayush gupta</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 30 January 2024</t>
-  </si>
-  <si>
-    <t>Dashing looks</t>
-  </si>
-  <si>
-    <t>FLIPKART</t>
-  </si>
-  <si>
-    <t>Sumit Yadav</t>
-  </si>
-  <si>
-    <t>Certified Buyer</t>
-  </si>
-  <si>
-    <t>20 Jan, 2024</t>
-  </si>
-  <si>
-    <t>boAt Enigma X700 with 1.52� AMOLED Display, BT Calling,Functional...</t>
-  </si>
-  <si>
-    <t>Shivendra Singh</t>
-  </si>
-  <si>
-    <t>UNKNOWN ERROR/INVALID LINK</t>
-  </si>
-  <si>
-    <t>Mustan Bharmal</t>
-  </si>
-  <si>
-    <t>Amit Maurya</t>
-  </si>
-  <si>
-    <t>19 Jan, 2024</t>
-  </si>
-  <si>
-    <t>Aaryan Singh</t>
-  </si>
-  <si>
-    <t>22 Jan, 2024</t>
-  </si>
-  <si>
-    <t>Rishabh Rai</t>
-  </si>
-  <si>
-    <t>21 Jan, 2024</t>
-  </si>
-  <si>
-    <t>P.g. Jain</t>
-  </si>
-  <si>
-    <t>25 Jan, 2024</t>
-  </si>
-  <si>
-    <t>Kartik Mehta</t>
-  </si>
-  <si>
-    <t>31 Jan, 2024</t>
-  </si>
-  <si>
-    <t>27 Jan, 2024</t>
-  </si>
-  <si>
-    <t>SOURAV Goyal</t>
-  </si>
-  <si>
-    <t>24 Jan, 2024</t>
-  </si>
-  <si>
-    <t>Varsha Goyal</t>
-  </si>
-  <si>
-    <t>04 Feb, 2024</t>
-  </si>
-  <si>
-    <t>Rehmat</t>
-  </si>
-  <si>
-    <t>05 Mar, 2024</t>
-  </si>
-  <si>
-    <t>review/B0CN2C26R9/R3KU02Q8XVIZAA</t>
-  </si>
-  <si>
-    <t>Deepak</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 17 March 2024</t>
-  </si>
-  <si>
-    <t>boAt Enigma Z20 Smart Watch with 1.51” HD Display, Luxurious Metal Body Design,Save Upto 250 Contacts,SOS, Password,Built-in Games,Voice Assistant,HR&amp;Sp02 Monitoring,IP68(Metal Black)</t>
-  </si>
-  <si>
-    <t>Superb watch!!</t>
-  </si>
-  <si>
-    <t>Raja Mondal</t>
-  </si>
-  <si>
-    <t>09 Mar, 2024</t>
-  </si>
-  <si>
-    <t>boAt Enigma Switch w/ Switchable Case, 1.39" HD Display, BT Calli...</t>
-  </si>
-  <si>
-    <t>14 Mar, 2024</t>
-  </si>
-  <si>
-    <t>Dhruv Choudhary</t>
-  </si>
-  <si>
-    <t>20 Mar, 2024</t>
-  </si>
-  <si>
-    <t>review/B0CN2RZR8M/R2PSY80EQL5HAR</t>
-  </si>
-  <si>
-    <t>Gulam Husen Sumra</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 4 March 2024</t>
-  </si>
-  <si>
-    <t>boAt Enigma Z20 Smart Watch with 1.51” HD Display, Luxurious Metal Body Design,Save Upto 250 Contacts,SOS, Password,Built-in Games,Voice Assistant,HR&amp;Sp02 Monitoring,IP68(Brown Leather)</t>
-  </si>
-  <si>
-    <t>Good product</t>
-  </si>
-  <si>
-    <t>2KU6V9G8KTQCO</t>
-  </si>
-  <si>
-    <t>Ratnaraj Creation</t>
-  </si>
-  <si>
-    <t>Awesome watch</t>
-  </si>
-  <si>
-    <t>review/B0CN2RZR8M/R70DTOGEKA1MP</t>
-  </si>
-  <si>
-    <t>Radha</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 14 March 2024</t>
-  </si>
-  <si>
-    <t>Best round dial watch</t>
-  </si>
-  <si>
-    <t>review/B0CN2C26R9/RBDNH8OE0RH51</t>
-  </si>
-  <si>
-    <t>Jagan Mohan Rao</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 29 February 2024</t>
-  </si>
-  <si>
-    <t>Worthy</t>
-  </si>
-  <si>
-    <t>R203OZTDNLTP0L</t>
-  </si>
-  <si>
-    <t>Sanjay saini</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 2 March 2024</t>
-  </si>
-  <si>
-    <t>Calling watch</t>
-  </si>
-  <si>
-    <t>2PWU2Q5W2BOUT</t>
-  </si>
-  <si>
-    <t>aditya sahu</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 12 March 2024</t>
-  </si>
-  <si>
-    <t>Best smart watch</t>
-  </si>
-  <si>
-    <t>R2VQ10C5PCGTRQ</t>
-  </si>
-  <si>
-    <t>Rishabh Kalia</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 26 March 2024</t>
-  </si>
-  <si>
-    <t>Achi watch h</t>
-  </si>
-  <si>
-    <t>Benoy Naskar</t>
-  </si>
-  <si>
-    <t>boAt Enigma Z20, 1.51 inch HD Display,BT Calling,Sturdy &amp; Luxurio...</t>
-  </si>
-  <si>
-    <t>Sakthi Kani</t>
-  </si>
-  <si>
-    <t>10 Mar, 2024</t>
-  </si>
-  <si>
-    <t>Shubham Gupta</t>
-  </si>
-  <si>
-    <t>neelesh dange</t>
-  </si>
-  <si>
-    <t>16 Mar, 2024</t>
-  </si>
-  <si>
-    <t>Neelay Rajani</t>
-  </si>
-  <si>
-    <t>11 Feb, 2024</t>
-  </si>
-  <si>
-    <t>R2I8V1XRULNGD4</t>
-  </si>
-  <si>
-    <t>Anuragkumar</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 8 February 2024</t>
-  </si>
-  <si>
-    <t>Lovely Birthday Gift!!</t>
-  </si>
-  <si>
-    <t>review/B0CN2JC9HC/R2MO1VSBLMTRIY</t>
-  </si>
-  <si>
-    <t>Shubham Kumar</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 12 February 2024</t>
-  </si>
-  <si>
-    <t>Perfect look</t>
-  </si>
-  <si>
-    <t>R13A0O5DR3K69</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 4 February 2024</t>
-  </si>
-  <si>
-    <t>Pure class and style!</t>
-  </si>
-  <si>
-    <t>Sangeeta Agarwal</t>
-  </si>
-  <si>
-    <t>08 Feb, 2024</t>
-  </si>
-  <si>
-    <t>review/B0CN2JC9HC/R2UR03QMLYCCNZ</t>
-  </si>
-  <si>
-    <t>Devendra</t>
-  </si>
-  <si>
-    <t>Blue color looks decent</t>
-  </si>
-  <si>
-    <t>review/B0CN2SYX6Q/R3BO2V4DXT7Z04</t>
-  </si>
-  <si>
-    <t>Ramesh Sharma</t>
-  </si>
-  <si>
-    <t>Quality is very very good Luxury Look smart watch..</t>
-  </si>
-  <si>
-    <t>review/B0CN2SYX6Q/R3HW83QANHQ6YR</t>
-  </si>
-  <si>
-    <t>Rinkesh Tunwal</t>
-  </si>
-  <si>
-    <t>Amazing Product</t>
-  </si>
-  <si>
-    <t>Puja Gupta</t>
-  </si>
-  <si>
-    <t>26 Jan, 2024</t>
-  </si>
-  <si>
-    <t>Sushmita Gupta</t>
-  </si>
-  <si>
-    <t>03 Feb, 2024</t>
-  </si>
-  <si>
-    <t>Ashok Rajani</t>
-  </si>
-  <si>
-    <t>Rut M.</t>
-  </si>
-  <si>
-    <t>24 Feb, 2024</t>
-  </si>
-  <si>
-    <t>review/B0CN2JC9HC/R18TFUZKE607WI</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 27 February 2024</t>
-  </si>
-  <si>
-    <t>Best purchase</t>
-  </si>
-  <si>
-    <t>review/B0CN2N8H94/R2JMJBLOZZ545Y</t>
-  </si>
-  <si>
-    <t>Looks stylish</t>
-  </si>
-  <si>
-    <t>review/B0CN2SYX6Q/R56K1MP42H412</t>
-  </si>
-  <si>
-    <t>pravesh mishra</t>
-  </si>
-  <si>
-    <t>Very stylish</t>
-  </si>
-  <si>
-    <t>review/B0CN2N8H94/R3R0ZY4TCHUHII</t>
-  </si>
-  <si>
-    <t>review/B0CN2SYX6Q/RX5O7XE2HTHX4</t>
-  </si>
-  <si>
-    <t>SHUBHAM SINGH</t>
-  </si>
-  <si>
-    <t>Wonderful gadget</t>
-  </si>
-  <si>
-    <t>Utkarsh Anand</t>
-  </si>
-  <si>
-    <t>27 Feb, 2024</t>
-  </si>
-  <si>
-    <t>Praveshmishra</t>
-  </si>
-  <si>
-    <t>Pratham Mishra</t>
-  </si>
-  <si>
-    <t>01 Mar, 2024</t>
-  </si>
-  <si>
-    <t>R2R9CNEIPPL4E3</t>
-  </si>
-  <si>
-    <t>Ranjeet Kumar</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 28 September 2023</t>
-  </si>
-  <si>
-    <t>boAt Enigma X500 Smart Watch w/ 1.43" AMOLED Display, Bluetooth Calling, Premium &amp; Luxurious Design, Functional Crown, 100+ Sports Modes, HR &amp; SpO2, IP68(Classic Silver)</t>
-  </si>
-  <si>
-    <t>Smooth Touch &amp; Luxurious Design</t>
-  </si>
-  <si>
-    <t>review/B0CN2N8H94/REZ2G9D1161CN</t>
-  </si>
-  <si>
-    <t>chirag</t>
-  </si>
-  <si>
-    <t>Reviewed in India on 9 February 2024</t>
-  </si>
-  <si>
-    <t>Truly the best</t>
-  </si>
-  <si>
-    <t>Priyanshu GUPTA</t>
-  </si>
-  <si>
-    <t>11 Mar, 2024</t>
   </si>
 </sst>
 </file>
@@ -14758,7 +14215,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14813,2323 +14272,361 @@
       <c r="A2" s="1" t="s">
         <v>4470</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4541</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4542</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4544</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4545</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4546</v>
-      </c>
-      <c r="J2">
-        <v>42</v>
-      </c>
-      <c r="K2" t="s">
-        <v>4547</v>
-      </c>
     </row>
     <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4471</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4548</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4549</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4550</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4551</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3">
-        <v>33</v>
-      </c>
-      <c r="K3" t="s">
-        <v>4547</v>
-      </c>
     </row>
     <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4472</v>
       </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4552</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4553</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>4550</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4545</v>
-      </c>
-      <c r="I4" t="s">
-        <v>4554</v>
-      </c>
-      <c r="J4">
-        <v>31</v>
-      </c>
-      <c r="K4" t="s">
-        <v>4547</v>
-      </c>
     </row>
     <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4473</v>
       </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4555</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4556</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>4557</v>
-      </c>
-      <c r="H5" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I5" t="s">
-        <v>4559</v>
-      </c>
-      <c r="J5">
-        <v>115</v>
-      </c>
-      <c r="K5" t="s">
-        <v>4547</v>
-      </c>
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4474</v>
       </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4560</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4561</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4562</v>
-      </c>
-      <c r="H6" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6">
-        <v>16</v>
-      </c>
-      <c r="K6" t="s">
-        <v>4563</v>
-      </c>
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4475</v>
       </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4564</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4565</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>4566</v>
-      </c>
-      <c r="H7" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I7" t="s">
-        <v>4567</v>
-      </c>
-      <c r="J7">
-        <v>33</v>
-      </c>
-      <c r="K7" t="s">
-        <v>4547</v>
-      </c>
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4476</v>
       </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4568</v>
-      </c>
-      <c r="D8" t="s">
-        <v>4569</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>4570</v>
-      </c>
-      <c r="H8" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I8" t="s">
-        <v>4571</v>
-      </c>
-      <c r="J8">
-        <v>22</v>
-      </c>
-      <c r="K8" t="s">
-        <v>4547</v>
-      </c>
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4477</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4572</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4573</v>
-      </c>
-      <c r="E9" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F9">
-        <v>5</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4562</v>
-      </c>
-      <c r="H9" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I9" t="s">
-        <v>4574</v>
-      </c>
-      <c r="J9">
-        <v>47</v>
-      </c>
-      <c r="K9" t="s">
-        <v>4547</v>
-      </c>
     </row>
     <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4478</v>
       </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4575</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4576</v>
-      </c>
-      <c r="E10" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-      <c r="G10" t="s">
-        <v>4550</v>
-      </c>
-      <c r="H10" t="s">
-        <v>4551</v>
-      </c>
-      <c r="I10" t="s">
-        <v>4577</v>
-      </c>
-      <c r="J10">
-        <v>67</v>
-      </c>
-      <c r="K10" t="s">
-        <v>4547</v>
-      </c>
     </row>
     <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4479</v>
       </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4578</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4579</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F11">
-        <v>5</v>
-      </c>
-      <c r="G11" t="s">
-        <v>4566</v>
-      </c>
-      <c r="H11" t="s">
-        <v>4551</v>
-      </c>
-      <c r="I11" t="s">
-        <v>4580</v>
-      </c>
-      <c r="J11">
-        <v>72</v>
-      </c>
-      <c r="K11" t="s">
-        <v>4547</v>
-      </c>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4480</v>
       </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4581</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4582</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F12">
-        <v>5</v>
-      </c>
-      <c r="G12" t="s">
-        <v>4550</v>
-      </c>
-      <c r="H12" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I12" t="s">
-        <v>4583</v>
-      </c>
-      <c r="J12">
-        <v>32</v>
-      </c>
-      <c r="K12" t="s">
-        <v>4547</v>
-      </c>
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4481</v>
       </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4584</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4585</v>
-      </c>
-      <c r="E13" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
-      <c r="G13" t="s">
-        <v>4586</v>
-      </c>
-      <c r="H13" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I13" t="s">
-        <v>4587</v>
-      </c>
-      <c r="J13">
-        <v>42</v>
-      </c>
-      <c r="K13" t="s">
-        <v>4547</v>
-      </c>
     </row>
     <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4482</v>
       </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4588</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4589</v>
-      </c>
-      <c r="E14" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-      <c r="G14" t="s">
-        <v>4590</v>
-      </c>
-      <c r="H14" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I14" t="s">
-        <v>4591</v>
-      </c>
-      <c r="J14">
-        <v>42</v>
-      </c>
-      <c r="K14" t="s">
-        <v>4563</v>
-      </c>
     </row>
     <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4483</v>
       </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D15" t="s">
-        <v>4593</v>
-      </c>
-      <c r="E15" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F15">
-        <v>5</v>
-      </c>
-      <c r="G15" t="s">
-        <v>4595</v>
-      </c>
-      <c r="H15" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J15">
-        <v>61</v>
-      </c>
-      <c r="K15" t="s">
-        <v>4563</v>
-      </c>
     </row>
     <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>4484</v>
       </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D16" t="s">
-        <v>4597</v>
-      </c>
-      <c r="E16" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F16">
-        <v>5</v>
-      </c>
-      <c r="G16" t="s">
-        <v>4595</v>
-      </c>
-      <c r="H16" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I16" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16">
-        <v>53</v>
-      </c>
-      <c r="K16" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>4521</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>4598</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>4522</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>4523</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>4524</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>4525</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>4485</v>
       </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D22" t="s">
-        <v>4599</v>
-      </c>
-      <c r="E22" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F22">
-        <v>5</v>
-      </c>
-      <c r="G22" t="s">
-        <v>4595</v>
-      </c>
-      <c r="H22" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I22" t="s">
-        <v>52</v>
-      </c>
-      <c r="J22">
-        <v>23</v>
-      </c>
-      <c r="K22" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>4486</v>
       </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4600</v>
-      </c>
-      <c r="E23" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F23">
-        <v>5</v>
-      </c>
-      <c r="G23" t="s">
-        <v>4601</v>
-      </c>
-      <c r="H23" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I23" t="s">
-        <v>42</v>
-      </c>
-      <c r="J23">
-        <v>48</v>
-      </c>
-      <c r="K23" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>4487</v>
       </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D24" t="s">
-        <v>4602</v>
-      </c>
-      <c r="E24" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F24">
-        <v>5</v>
-      </c>
-      <c r="G24" t="s">
-        <v>4603</v>
-      </c>
-      <c r="H24" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I24" t="s">
-        <v>91</v>
-      </c>
-      <c r="J24">
-        <v>57</v>
-      </c>
-      <c r="K24" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>4488</v>
       </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1865</v>
-      </c>
-      <c r="E25" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
-      </c>
-      <c r="G25" t="s">
-        <v>4603</v>
-      </c>
-      <c r="H25" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I25" t="s">
-        <v>42</v>
-      </c>
-      <c r="J25">
-        <v>61</v>
-      </c>
-      <c r="K25" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>4489</v>
       </c>
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4604</v>
-      </c>
-      <c r="E26" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F26">
-        <v>5</v>
-      </c>
-      <c r="G26" t="s">
-        <v>4605</v>
-      </c>
-      <c r="H26" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I26" t="s">
-        <v>60</v>
-      </c>
-      <c r="J26">
-        <v>128</v>
-      </c>
-      <c r="K26" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>4490</v>
       </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4606</v>
-      </c>
-      <c r="E27" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F27">
-        <v>5</v>
-      </c>
-      <c r="G27" t="s">
-        <v>4607</v>
-      </c>
-      <c r="H27" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I27" t="s">
-        <v>42</v>
-      </c>
-      <c r="J27">
-        <v>72</v>
-      </c>
-      <c r="K27" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>4491</v>
       </c>
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D28" t="s">
-        <v>4608</v>
-      </c>
-      <c r="E28" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F28">
-        <v>5</v>
-      </c>
-      <c r="G28" t="s">
-        <v>4609</v>
-      </c>
-      <c r="H28" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I28" t="s">
-        <v>41</v>
-      </c>
-      <c r="J28">
-        <v>22</v>
-      </c>
-      <c r="K28" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>4492</v>
       </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1140</v>
-      </c>
-      <c r="E29" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F29">
-        <v>5</v>
-      </c>
-      <c r="G29" t="s">
-        <v>4610</v>
-      </c>
-      <c r="H29" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I29" t="s">
-        <v>67</v>
-      </c>
-      <c r="J29">
-        <v>15</v>
-      </c>
-      <c r="K29" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>4493</v>
       </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D30" t="s">
-        <v>4611</v>
-      </c>
-      <c r="E30" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F30">
-        <v>5</v>
-      </c>
-      <c r="G30" t="s">
-        <v>4612</v>
-      </c>
-      <c r="H30" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I30" t="s">
-        <v>91</v>
-      </c>
-      <c r="J30">
-        <v>40</v>
-      </c>
-      <c r="K30" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>4494</v>
       </c>
-      <c r="B31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D31" t="s">
-        <v>4613</v>
-      </c>
-      <c r="E31" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F31">
-        <v>5</v>
-      </c>
-      <c r="G31" t="s">
-        <v>4614</v>
-      </c>
-      <c r="H31" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J31">
-        <v>58</v>
-      </c>
-      <c r="K31" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>4495</v>
       </c>
-      <c r="B32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D32" t="s">
-        <v>4615</v>
-      </c>
-      <c r="E32" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F32">
-        <v>5</v>
-      </c>
-      <c r="G32" t="s">
-        <v>4616</v>
-      </c>
-      <c r="H32" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I32" t="s">
-        <v>41</v>
-      </c>
-      <c r="J32">
-        <v>22</v>
-      </c>
-      <c r="K32" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>4526</v>
       </c>
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4617</v>
-      </c>
-      <c r="D33" t="s">
-        <v>4618</v>
-      </c>
-      <c r="E33" t="s">
-        <v>4563</v>
-      </c>
-      <c r="F33">
-        <v>5</v>
-      </c>
-      <c r="G33" t="s">
-        <v>4619</v>
-      </c>
-      <c r="H33" t="s">
-        <v>4620</v>
-      </c>
-      <c r="I33" t="s">
-        <v>4621</v>
-      </c>
-      <c r="J33">
-        <v>33</v>
-      </c>
-      <c r="K33" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>4527</v>
       </c>
-      <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D34" t="s">
-        <v>4622</v>
-      </c>
-      <c r="E34" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F34">
-        <v>5</v>
-      </c>
-      <c r="G34" t="s">
-        <v>4623</v>
-      </c>
-      <c r="H34" t="s">
-        <v>4624</v>
-      </c>
-      <c r="I34" t="s">
-        <v>55</v>
-      </c>
-      <c r="J34">
-        <v>45</v>
-      </c>
-      <c r="K34" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>4528</v>
       </c>
-      <c r="B35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D35" t="s">
-        <v>4600</v>
-      </c>
-      <c r="E35" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F35">
-        <v>5</v>
-      </c>
-      <c r="G35" t="s">
-        <v>4625</v>
-      </c>
-      <c r="H35" t="s">
-        <v>4624</v>
-      </c>
-      <c r="I35" t="s">
-        <v>60</v>
-      </c>
-      <c r="J35">
-        <v>80</v>
-      </c>
-      <c r="K35" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>4529</v>
       </c>
-      <c r="B36" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D36" t="s">
-        <v>4626</v>
-      </c>
-      <c r="E36" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F36">
-        <v>5</v>
-      </c>
-      <c r="G36" t="s">
-        <v>4627</v>
-      </c>
-      <c r="H36" t="s">
-        <v>4624</v>
-      </c>
-      <c r="I36" t="s">
-        <v>252</v>
-      </c>
-      <c r="J36">
-        <v>44</v>
-      </c>
-      <c r="K36" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>4530</v>
       </c>
-      <c r="B37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4628</v>
-      </c>
-      <c r="D37" t="s">
-        <v>4629</v>
-      </c>
-      <c r="E37" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F37">
-        <v>5</v>
-      </c>
-      <c r="G37" t="s">
-        <v>4630</v>
-      </c>
-      <c r="H37" t="s">
-        <v>4631</v>
-      </c>
-      <c r="I37" t="s">
-        <v>4632</v>
-      </c>
-      <c r="J37">
-        <v>18</v>
-      </c>
-      <c r="K37" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>4531</v>
       </c>
-      <c r="B38" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" t="s">
-        <v>4633</v>
-      </c>
-      <c r="D38" t="s">
-        <v>4634</v>
-      </c>
-      <c r="E38" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F38">
-        <v>5</v>
-      </c>
-      <c r="G38" t="s">
-        <v>4630</v>
-      </c>
-      <c r="H38" t="s">
-        <v>4631</v>
-      </c>
-      <c r="I38" t="s">
-        <v>4635</v>
-      </c>
-      <c r="J38">
-        <v>66</v>
-      </c>
-      <c r="K38" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>4532</v>
       </c>
-      <c r="B39" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" t="s">
-        <v>4636</v>
-      </c>
-      <c r="D39" t="s">
-        <v>4637</v>
-      </c>
-      <c r="E39" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F39">
-        <v>5</v>
-      </c>
-      <c r="G39" t="s">
-        <v>4638</v>
-      </c>
-      <c r="H39" t="s">
-        <v>4631</v>
-      </c>
-      <c r="I39" t="s">
-        <v>4639</v>
-      </c>
-      <c r="J39">
-        <v>59</v>
-      </c>
-      <c r="K39" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>4533</v>
       </c>
-      <c r="B40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" t="s">
-        <v>4640</v>
-      </c>
-      <c r="D40" t="s">
-        <v>4641</v>
-      </c>
-      <c r="E40" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F40">
-        <v>5</v>
-      </c>
-      <c r="G40" t="s">
-        <v>4642</v>
-      </c>
-      <c r="H40" t="s">
-        <v>4620</v>
-      </c>
-      <c r="I40" t="s">
-        <v>4643</v>
-      </c>
-      <c r="J40">
-        <v>22</v>
-      </c>
-      <c r="K40" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>4534</v>
       </c>
-      <c r="B41" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" t="s">
-        <v>4644</v>
-      </c>
-      <c r="D41" t="s">
-        <v>4645</v>
-      </c>
-      <c r="E41" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F41">
-        <v>5</v>
-      </c>
-      <c r="G41" t="s">
-        <v>4646</v>
-      </c>
-      <c r="H41" t="s">
-        <v>4620</v>
-      </c>
-      <c r="I41" t="s">
-        <v>4647</v>
-      </c>
-      <c r="J41">
-        <v>27</v>
-      </c>
-      <c r="K41" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>4535</v>
       </c>
-      <c r="B42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C42" t="s">
-        <v>4648</v>
-      </c>
-      <c r="D42" t="s">
-        <v>4649</v>
-      </c>
-      <c r="E42" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F42">
-        <v>5</v>
-      </c>
-      <c r="G42" t="s">
-        <v>4650</v>
-      </c>
-      <c r="H42" t="s">
-        <v>4620</v>
-      </c>
-      <c r="I42" t="s">
-        <v>4651</v>
-      </c>
-      <c r="J42">
-        <v>78</v>
-      </c>
-      <c r="K42" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>4536</v>
       </c>
-      <c r="B43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" t="s">
-        <v>4652</v>
-      </c>
-      <c r="D43" t="s">
-        <v>4653</v>
-      </c>
-      <c r="E43" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F43">
-        <v>5</v>
-      </c>
-      <c r="G43" t="s">
-        <v>4654</v>
-      </c>
-      <c r="H43" t="s">
-        <v>4620</v>
-      </c>
-      <c r="I43" t="s">
-        <v>4655</v>
-      </c>
-      <c r="J43">
-        <v>34</v>
-      </c>
-      <c r="K43" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>4537</v>
       </c>
-      <c r="B44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D44" t="s">
-        <v>4656</v>
-      </c>
-      <c r="E44" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F44">
-        <v>5</v>
-      </c>
-      <c r="G44" t="s">
-        <v>4616</v>
-      </c>
-      <c r="H44" t="s">
-        <v>4657</v>
-      </c>
-      <c r="I44" t="s">
-        <v>67</v>
-      </c>
-      <c r="J44">
-        <v>65</v>
-      </c>
-      <c r="K44" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>4538</v>
       </c>
-      <c r="B45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D45" t="s">
-        <v>4658</v>
-      </c>
-      <c r="E45" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F45">
-        <v>5</v>
-      </c>
-      <c r="G45" t="s">
-        <v>4659</v>
-      </c>
-      <c r="H45" t="s">
-        <v>4657</v>
-      </c>
-      <c r="I45" t="s">
-        <v>67</v>
-      </c>
-      <c r="J45">
-        <v>39</v>
-      </c>
-      <c r="K45" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>4539</v>
       </c>
-      <c r="B46" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D46" t="s">
-        <v>4660</v>
-      </c>
-      <c r="E46" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F46">
-        <v>5</v>
-      </c>
-      <c r="G46" t="s">
-        <v>4659</v>
-      </c>
-      <c r="H46" t="s">
-        <v>4657</v>
-      </c>
-      <c r="I46" t="s">
-        <v>54</v>
-      </c>
-      <c r="J46">
-        <v>53</v>
-      </c>
-      <c r="K46" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>4540</v>
       </c>
-      <c r="B47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D47" t="s">
-        <v>4661</v>
-      </c>
-      <c r="E47" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F47">
-        <v>5</v>
-      </c>
-      <c r="G47" t="s">
-        <v>4662</v>
-      </c>
-      <c r="H47" t="s">
-        <v>4657</v>
-      </c>
-      <c r="I47" t="s">
-        <v>60</v>
-      </c>
-      <c r="J47">
-        <v>41</v>
-      </c>
-      <c r="K47" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>4496</v>
       </c>
-      <c r="B48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D48" t="s">
-        <v>4663</v>
-      </c>
-      <c r="E48" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F48">
-        <v>5</v>
-      </c>
-      <c r="G48" t="s">
-        <v>4664</v>
-      </c>
-      <c r="H48" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I48" t="s">
-        <v>252</v>
-      </c>
-      <c r="J48">
-        <v>39</v>
-      </c>
-      <c r="K48" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>4497</v>
       </c>
-      <c r="B49" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" t="s">
-        <v>4665</v>
-      </c>
-      <c r="D49" t="s">
-        <v>4666</v>
-      </c>
-      <c r="E49" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F49">
-        <v>5</v>
-      </c>
-      <c r="G49" t="s">
-        <v>4667</v>
-      </c>
-      <c r="H49" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I49" t="s">
-        <v>4668</v>
-      </c>
-      <c r="J49">
-        <v>121</v>
-      </c>
-      <c r="K49" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>4498</v>
       </c>
-      <c r="B50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C50" t="s">
-        <v>4669</v>
-      </c>
-      <c r="D50" t="s">
-        <v>4670</v>
-      </c>
-      <c r="E50" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F50">
-        <v>5</v>
-      </c>
-      <c r="G50" t="s">
-        <v>4671</v>
-      </c>
-      <c r="H50" t="s">
-        <v>4545</v>
-      </c>
-      <c r="I50" t="s">
-        <v>4672</v>
-      </c>
-      <c r="J50">
-        <v>45</v>
-      </c>
-      <c r="K50" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>4499</v>
       </c>
-      <c r="B51" t="s">
-        <v>29</v>
-      </c>
-      <c r="C51" t="s">
-        <v>4673</v>
-      </c>
-      <c r="D51" t="s">
-        <v>31</v>
-      </c>
-      <c r="E51" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F51">
-        <v>5</v>
-      </c>
-      <c r="G51" t="s">
-        <v>4674</v>
-      </c>
-      <c r="H51" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I51" t="s">
-        <v>4675</v>
-      </c>
-      <c r="J51">
-        <v>93</v>
-      </c>
-      <c r="K51" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>4500</v>
       </c>
-      <c r="B52" t="s">
-        <v>29</v>
-      </c>
-      <c r="C52" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D52" t="s">
-        <v>4676</v>
-      </c>
-      <c r="E52" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F52">
-        <v>5</v>
-      </c>
-      <c r="G52" t="s">
-        <v>4677</v>
-      </c>
-      <c r="H52" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I52" t="s">
-        <v>67</v>
-      </c>
-      <c r="J52">
-        <v>53</v>
-      </c>
-      <c r="K52" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>4501</v>
       </c>
-      <c r="B53" t="s">
-        <v>29</v>
-      </c>
-      <c r="C53" t="s">
-        <v>4678</v>
-      </c>
-      <c r="D53" t="s">
-        <v>4679</v>
-      </c>
-      <c r="E53" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F53">
-        <v>5</v>
-      </c>
-      <c r="G53" t="s">
-        <v>4550</v>
-      </c>
-      <c r="H53" t="s">
-        <v>4545</v>
-      </c>
-      <c r="I53" t="s">
-        <v>4680</v>
-      </c>
-      <c r="J53">
-        <v>21</v>
-      </c>
-      <c r="K53" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>4502</v>
       </c>
-      <c r="B54" t="s">
-        <v>29</v>
-      </c>
-      <c r="C54" t="s">
-        <v>4681</v>
-      </c>
-      <c r="D54" t="s">
-        <v>4682</v>
-      </c>
-      <c r="E54" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F54">
-        <v>5</v>
-      </c>
-      <c r="G54" t="s">
-        <v>4550</v>
-      </c>
-      <c r="H54" t="s">
-        <v>4551</v>
-      </c>
-      <c r="I54" t="s">
-        <v>4683</v>
-      </c>
-      <c r="J54">
-        <v>45</v>
-      </c>
-      <c r="K54" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>4503</v>
       </c>
-      <c r="B55" t="s">
-        <v>29</v>
-      </c>
-      <c r="C55" t="s">
-        <v>4684</v>
-      </c>
-      <c r="D55" t="s">
-        <v>4685</v>
-      </c>
-      <c r="E55" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F55">
-        <v>5</v>
-      </c>
-      <c r="G55" t="s">
-        <v>4590</v>
-      </c>
-      <c r="H55" t="s">
-        <v>4551</v>
-      </c>
-      <c r="I55" t="s">
-        <v>4686</v>
-      </c>
-      <c r="J55">
-        <v>43</v>
-      </c>
-      <c r="K55" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>4504</v>
       </c>
-      <c r="B56" t="s">
-        <v>29</v>
-      </c>
-      <c r="C56" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D56" t="s">
-        <v>4687</v>
-      </c>
-      <c r="E56" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F56">
-        <v>5</v>
-      </c>
-      <c r="G56" t="s">
-        <v>4688</v>
-      </c>
-      <c r="H56" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I56" t="s">
-        <v>39</v>
-      </c>
-      <c r="J56">
-        <v>73</v>
-      </c>
-      <c r="K56" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>4505</v>
       </c>
-      <c r="B57" t="s">
-        <v>29</v>
-      </c>
-      <c r="C57" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D57" t="s">
-        <v>4689</v>
-      </c>
-      <c r="E57" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F57">
-        <v>5</v>
-      </c>
-      <c r="G57" t="s">
-        <v>4690</v>
-      </c>
-      <c r="H57" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I57" t="s">
-        <v>67</v>
-      </c>
-      <c r="J57">
-        <v>67</v>
-      </c>
-      <c r="K57" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>4506</v>
       </c>
-      <c r="B58" t="s">
-        <v>29</v>
-      </c>
-      <c r="C58" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D58" t="s">
-        <v>4691</v>
-      </c>
-      <c r="E58" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F58">
-        <v>5</v>
-      </c>
-      <c r="G58" t="s">
-        <v>4609</v>
-      </c>
-      <c r="H58" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I58" t="s">
-        <v>55</v>
-      </c>
-      <c r="J58">
-        <v>33</v>
-      </c>
-      <c r="K58" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>4507</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="5"/>
+    </row>
+    <row r="60" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>4508</v>
       </c>
-      <c r="B60" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D60" t="s">
-        <v>4692</v>
-      </c>
-      <c r="E60" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F60">
-        <v>5</v>
-      </c>
-      <c r="G60" t="s">
-        <v>4693</v>
-      </c>
-      <c r="H60" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I60" t="s">
-        <v>41</v>
-      </c>
-      <c r="J60">
-        <v>11</v>
-      </c>
-      <c r="K60" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>4509</v>
       </c>
-      <c r="B61" t="s">
-        <v>29</v>
-      </c>
-      <c r="C61" t="s">
-        <v>4694</v>
-      </c>
-      <c r="D61" t="s">
-        <v>1346</v>
-      </c>
-      <c r="E61" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F61">
-        <v>5</v>
-      </c>
-      <c r="G61" t="s">
-        <v>4695</v>
-      </c>
-      <c r="H61" t="s">
-        <v>4545</v>
-      </c>
-      <c r="I61" t="s">
-        <v>4696</v>
-      </c>
-      <c r="J61">
-        <v>41</v>
-      </c>
-      <c r="K61" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>4510</v>
       </c>
-      <c r="B62" t="s">
-        <v>29</v>
-      </c>
-      <c r="C62" t="s">
-        <v>4697</v>
-      </c>
-      <c r="D62" t="s">
-        <v>34</v>
-      </c>
-      <c r="E62" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F62">
-        <v>5</v>
-      </c>
-      <c r="G62" t="s">
-        <v>4695</v>
-      </c>
-      <c r="H62" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I62" t="s">
-        <v>4698</v>
-      </c>
-      <c r="J62">
-        <v>44</v>
-      </c>
-      <c r="K62" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>4511</v>
       </c>
-      <c r="B63" t="s">
-        <v>29</v>
-      </c>
-      <c r="C63" t="s">
-        <v>4699</v>
-      </c>
-      <c r="D63" t="s">
-        <v>4700</v>
-      </c>
-      <c r="E63" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F63">
-        <v>5</v>
-      </c>
-      <c r="G63" t="s">
-        <v>4695</v>
-      </c>
-      <c r="H63" t="s">
-        <v>4551</v>
-      </c>
-      <c r="I63" t="s">
-        <v>4701</v>
-      </c>
-      <c r="J63">
-        <v>51</v>
-      </c>
-      <c r="K63" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:2" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>4512</v>
       </c>
-      <c r="B64" t="s">
-        <v>29</v>
-      </c>
-      <c r="C64" t="s">
-        <v>4702</v>
-      </c>
-      <c r="D64" t="s">
-        <v>1340</v>
-      </c>
-      <c r="E64" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F64">
-        <v>5</v>
-      </c>
-      <c r="G64" t="s">
-        <v>4695</v>
-      </c>
-      <c r="H64" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I64" t="s">
-        <v>4698</v>
-      </c>
-      <c r="J64">
-        <v>44</v>
-      </c>
-      <c r="K64" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>4513</v>
       </c>
-      <c r="B65" t="s">
-        <v>29</v>
-      </c>
-      <c r="C65" t="s">
-        <v>4703</v>
-      </c>
-      <c r="D65" t="s">
-        <v>4704</v>
-      </c>
-      <c r="E65" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F65">
-        <v>5</v>
-      </c>
-      <c r="G65" t="s">
-        <v>4695</v>
-      </c>
-      <c r="H65" t="s">
-        <v>4551</v>
-      </c>
-      <c r="I65" t="s">
-        <v>4705</v>
-      </c>
-      <c r="J65">
-        <v>50</v>
-      </c>
-      <c r="K65" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>4514</v>
       </c>
-      <c r="B66" t="s">
-        <v>29</v>
-      </c>
-      <c r="C66" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D66" t="s">
-        <v>4706</v>
-      </c>
-      <c r="E66" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F66">
-        <v>5</v>
-      </c>
-      <c r="G66" t="s">
-        <v>4707</v>
-      </c>
-      <c r="H66" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I66" t="s">
-        <v>49</v>
-      </c>
-      <c r="J66">
-        <v>42</v>
-      </c>
-      <c r="K66" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>4515</v>
       </c>
-      <c r="B67" t="s">
-        <v>29</v>
-      </c>
-      <c r="C67" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D67" t="s">
-        <v>4708</v>
-      </c>
-      <c r="E67" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F67">
-        <v>5</v>
-      </c>
-      <c r="G67" t="s">
-        <v>4707</v>
-      </c>
-      <c r="H67" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I67" t="s">
-        <v>60</v>
-      </c>
-      <c r="J67">
-        <v>54</v>
-      </c>
-      <c r="K67" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>4516</v>
       </c>
-      <c r="B68" t="s">
-        <v>29</v>
-      </c>
-      <c r="C68" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D68" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F68">
-        <v>5</v>
-      </c>
-      <c r="G68" t="s">
-        <v>4707</v>
-      </c>
-      <c r="H68" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I68" t="s">
-        <v>32</v>
-      </c>
-      <c r="J68">
-        <v>40</v>
-      </c>
-      <c r="K68" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>4517</v>
       </c>
-      <c r="B69" t="s">
-        <v>29</v>
-      </c>
-      <c r="C69" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D69" t="s">
-        <v>4709</v>
-      </c>
-      <c r="E69" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F69">
-        <v>5</v>
-      </c>
-      <c r="G69" t="s">
-        <v>4710</v>
-      </c>
-      <c r="H69" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I69" t="s">
-        <v>139</v>
-      </c>
-      <c r="J69">
-        <v>11</v>
-      </c>
-      <c r="K69" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>4518</v>
       </c>
-      <c r="B70" t="s">
-        <v>29</v>
-      </c>
-      <c r="C70" t="s">
-        <v>4711</v>
-      </c>
-      <c r="D70" t="s">
-        <v>4712</v>
-      </c>
-      <c r="E70" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F70">
-        <v>5</v>
-      </c>
-      <c r="G70" t="s">
-        <v>4713</v>
-      </c>
-      <c r="H70" t="s">
-        <v>4714</v>
-      </c>
-      <c r="I70" t="s">
-        <v>4715</v>
-      </c>
-      <c r="J70">
-        <v>44</v>
-      </c>
-      <c r="K70" t="s">
-        <v>4547</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>4519</v>
       </c>
-      <c r="B71" t="s">
-        <v>29</v>
-      </c>
-      <c r="C71" t="s">
-        <v>4716</v>
-      </c>
-      <c r="D71" t="s">
-        <v>4717</v>
-      </c>
-      <c r="E71" t="s">
-        <v>4543</v>
-      </c>
-      <c r="F71">
-        <v>4</v>
-      </c>
-      <c r="G71" t="s">
-        <v>4718</v>
-      </c>
-      <c r="H71" t="s">
-        <v>4558</v>
-      </c>
-      <c r="I71" t="s">
-        <v>4719</v>
-      </c>
-      <c r="J71">
-        <v>46</v>
-      </c>
-      <c r="K71" t="s">
-        <v>4563</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>4520</v>
-      </c>
-      <c r="B72" t="s">
-        <v>29</v>
-      </c>
-      <c r="C72" t="s">
-        <v>4592</v>
-      </c>
-      <c r="D72" t="s">
-        <v>4720</v>
-      </c>
-      <c r="E72" t="s">
-        <v>4594</v>
-      </c>
-      <c r="F72">
-        <v>5</v>
-      </c>
-      <c r="G72" t="s">
-        <v>4721</v>
-      </c>
-      <c r="H72" t="s">
-        <v>4596</v>
-      </c>
-      <c r="I72" t="s">
-        <v>54</v>
-      </c>
-      <c r="J72">
-        <v>51</v>
-      </c>
-      <c r="K72" t="s">
-        <v>4563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>